<commit_message>
add note about spring init
</commit_message>
<xml_diff>
--- a/com.w/main/note/时间管理计划.xlsx
+++ b/com.w/main/note/时间管理计划.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wp\wpNote\com.w\main\note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07900955-5F3C-4C28-8445-92CBF7D2457E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E9C150-06CB-4DEE-8430-9D9CF201EC8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1164" yWindow="1356" windowWidth="16608" windowHeight="10524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="759">
   <si>
     <t>星期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2648,6 +2648,108 @@
   </si>
   <si>
     <t>平静</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.25</t>
+  </si>
+  <si>
+    <t>2.26</t>
+  </si>
+  <si>
+    <t>2.27</t>
+  </si>
+  <si>
+    <t>2.28</t>
+  </si>
+  <si>
+    <t>3.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>3.11</t>
+  </si>
+  <si>
+    <t>3.12</t>
+  </si>
+  <si>
+    <t>3.13</t>
+  </si>
+  <si>
+    <t>3.14</t>
+  </si>
+  <si>
+    <t>3.15</t>
+  </si>
+  <si>
+    <t>3.16</t>
+  </si>
+  <si>
+    <t>回学校，拍毕业图像采集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.17</t>
+  </si>
+  <si>
+    <t>3.18</t>
+  </si>
+  <si>
+    <t>3.19</t>
+  </si>
+  <si>
+    <t>回北京</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>投递简历，B站，Keep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.20</t>
+  </si>
+  <si>
+    <t>3.21</t>
+  </si>
+  <si>
+    <t>3.22</t>
+  </si>
+  <si>
+    <t>3.23</t>
+  </si>
+  <si>
+    <t>编码能力需要提升</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海康笔试，用友面试</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3778,10 +3880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFCEDE24-A154-473C-9FA3-EA46E98C807D}">
-  <dimension ref="A1:R318"/>
+  <dimension ref="A1:R345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E299" workbookViewId="0">
-      <selection activeCell="F318" sqref="F318"/>
+    <sheetView tabSelected="1" topLeftCell="A332" workbookViewId="0">
+      <selection activeCell="E342" sqref="E342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8624,6 +8726,240 @@
       </c>
       <c r="G318">
         <v>0.25</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>317</v>
+      </c>
+      <c r="B319" s="8" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>318</v>
+      </c>
+      <c r="B320" s="8" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>319</v>
+      </c>
+      <c r="B321" s="8" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>320</v>
+      </c>
+      <c r="B322" s="8" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>321</v>
+      </c>
+      <c r="B323" s="8" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>322</v>
+      </c>
+      <c r="B324" s="8" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>323</v>
+      </c>
+      <c r="B325" s="8" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>324</v>
+      </c>
+      <c r="B326" s="8" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>325</v>
+      </c>
+      <c r="B327" s="8" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>326</v>
+      </c>
+      <c r="B328" s="8" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>327</v>
+      </c>
+      <c r="B329" s="8" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>328</v>
+      </c>
+      <c r="B330" s="8" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>329</v>
+      </c>
+      <c r="B331" s="8" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>330</v>
+      </c>
+      <c r="B332" s="8" t="s">
+        <v>740</v>
+      </c>
+      <c r="C332" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>331</v>
+      </c>
+      <c r="B333" s="8" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>332</v>
+      </c>
+      <c r="B334" s="8" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>333</v>
+      </c>
+      <c r="B335" s="8" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>334</v>
+      </c>
+      <c r="B336" s="8" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>335</v>
+      </c>
+      <c r="B337" s="8" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>336</v>
+      </c>
+      <c r="B338" s="8" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>337</v>
+      </c>
+      <c r="B339" s="8" t="s">
+        <v>748</v>
+      </c>
+      <c r="C339" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>338</v>
+      </c>
+      <c r="B340" s="8" t="s">
+        <v>749</v>
+      </c>
+      <c r="C340" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>339</v>
+      </c>
+      <c r="B341" s="8" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>340</v>
+      </c>
+      <c r="B342" s="8" t="s">
+        <v>753</v>
+      </c>
+      <c r="C342" t="s">
+        <v>758</v>
+      </c>
+      <c r="D342" t="s">
+        <v>497</v>
+      </c>
+      <c r="E342" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>341</v>
+      </c>
+      <c r="B343" s="8" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>342</v>
+      </c>
+      <c r="B344" s="8" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>343</v>
+      </c>
+      <c r="B345" s="8" t="s">
+        <v>756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>